<commit_message>
update main and new scripts
</commit_message>
<xml_diff>
--- a/results/training_set_prediction.xlsx
+++ b/results/training_set_prediction.xlsx
@@ -453,24 +453,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SMWSGMWRRKLKKLRNALKKKLKGEK</t>
+          <t>FNQWTTWCYHHMVPYCDYCHFKR</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>KSYGNGVHCNKKKCWVDWGSAISTIGNNSAANWATGGAAGWKS</t>
+          <t>MEANSRVMVRVLLLALVVQVTLSQHWSYGWLPGGKRSVGELEATIRMMGTGEVVSLPEEASAQTQERLRPYNVINDDSSHFDRKKRSPNK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -492,11 +492,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>QQDYTGWFDF</t>
+          <t>SILSGNFGVGKKIVCGLSGLC</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -505,20 +505,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WFDVDLNNIQGWIAITDGLFLEEYNKACWSCQGGPQTIHMCIHDVLIHQPFTPHAAL</t>
+          <t>ASNQDFMRF</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GLFNVFKGLKTAGKHVAGSLLNQLKCKVSGGC</t>
+          <t>LFKLLGKIIHHVGNFVHGFSHVF</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -531,20 +531,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VTSYTLSDVVPLKDVVPEWVRIGFSATPGAEYAAHEVLSWSFHSELSGTSSKQ</t>
+          <t>RPRPNYRPRPIYRP</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SILSGNFGVGKKIVCGLSGLC</t>
+          <t>MKTFSVAVAVAVVLAFICTQESSALPVTGIEELVEPVSSDNNDNHQGLPVELRERLVNIRKKRAPTDCIPYCYPTGDGFHCGVTCRF</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -570,11 +570,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GGYYCPFRQDKCHRHCRSFGRKAGYCGGFLKKTCICV</t>
+          <t>KFYFTFPS</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
@@ -583,7 +583,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ITSVSWCTPGCTSEGGGSGCSHCC</t>
+          <t>GILSTFKGLAKGVAKDLAGNLLDKFKCKITGC</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -596,33 +596,33 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MEANSRVMVRVLLLALVVQVTLSQHWSYGWLPGGKRSVGELEATIRMMGTGEVVSLPEEASAQTQERLRPYNVINDDSSHFDRKKRSPNK</t>
+          <t>KSYGNGVHCNKKKCWVDWGSAISTIGNNSAANWATGGAAGWKS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MHLSPQEKDKLLIVTAALLAERRLNRGLKLNHPEAVAWLSFLVLEGARDGKSVAELMQEGTTWLSRNQVMDGIPELVQEVQIEAVFPDGTKLVTLHDPIR</t>
+          <t>MDGKAPAAFVEPGEFNEVMKRLDQIDEKVEFVNSEVAQRIGKKVGRDIGILYGGVIGLLLFLIYVQISSMFM</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RPRPNYRPRPIYRP</t>
+          <t>RSALSCQMCELVVKKYEGSADKDANVIKKDFDAECKKLFHTIPFGTRECDHYVNSKVDPIIHELEGGTAPKDVCTKLNECP</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MPKLAVVLLVLLILPLSYFDAAGGQAVQWDRRGNGLARYLQRGDRDVRECQVDTPGSSWGKCCMTRMCGTMCCSRSVCTCVYHWRRGHGCSCPG</t>
+          <t>NGMYFFYLNSIPAEMGRQCCAHADTYIYAMERVMFVPQFVCNSGIWTGHWKPAFRLPECYSTPWWKKS</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -648,46 +648,46 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LFKLLGKIIHHVGNFVHGFSHVF</t>
+          <t>MHLSPQEKDKLLIVTAALLAERRLNRGLKLNHPEAVAWLSFLVLEGARDGKSVAELMQEGTTWLSRNQVMDGIPELVQEVQIEAVFPDGTKLVTLHDPIR</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ASNQDFMRF</t>
+          <t>WFDVDLNNIQGWIAITDGLFLEEYNKACWSCQGGPQTIHMCIHDVLIHQPFTPHAAL</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MKTFSVAVAVAVVLAFICTQESSALPVTGIEELVEPVSSDNNDNHQGLPVELRERLVNIRKKRAPTDCIPYCYPTGDGFHCGVTCRF</t>
+          <t>GGYYCPFRQDKCHRHCRSFGRKAGYCGGFLKKTCICV</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TLEVCPQQHYCYDDHATSLYQPLFPQGPRMDINIWLWLSMPLNLHELRIWCAEDNGVWPHNSWKNPRKCNVVVTQPDTPPGS</t>
+          <t>MPKLAVVLLVLLILPLSYFDAAGGQAVQWDRRGNGLARYLQRGDRDVRECQVDTPGSSWGKCCMTRMCGTMCCSRSVCTCVYHWRRGHGCSCPG</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -707,43 +707,43 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MDGKAPAAFVEPGEFNEVMKRLDQIDEKVEFVNSEVAQRIGKKVGRDIGILYGGVIGLLLFLIYVQISSMFM</t>
+          <t>QQDYTGWFDF</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>FNQWTTWCYHHMVPYCDYCHFKR</t>
+          <t>GLFNVFKGLKTAGKHVAGSLLNQLKCKVSGGC</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>FLPAIAGMAAKFLPKIFCAISKKC</t>
+          <t>LICVKEKFLFSETTETCPDGQNVCFNQAHLIYPGKYKRTRGCAATCPKLQNRDVIFCCSTDKCNL</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
@@ -752,7 +752,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GILSTFKGLAKGVAKDLAGNLLDKFKCKITGC</t>
+          <t>FLPAIAGMAAKFLPKIFCAISKKC</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -765,24 +765,24 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KFYFTFPS</t>
+          <t>SMWSGMWRRKLKKLRNALKKKLKGEK</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RSALSCQMCELVVKKYEGSADKDANVIKKDFDAECKKLFHTIPFGTRECDHYVNSKVDPIIHELEGGTAPKDVCTKLNECP</t>
+          <t>VTSYTLSDVVPLKDVVPEWVRIGFSATPGAEYAAHEVLSWSFHSELSGTSSKQ</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -791,7 +791,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NGMYFFYLNSIPAEMGRQCCAHADTYIYAMERVMFVPQFVCNSGIWTGHWKPAFRLPECYSTPWWKKS</t>
+          <t>TLEVCPQQHYCYDDHATSLYQPLFPQGPRMDINIWLWLSMPLNLHELRIWCAEDNGVWPHNSWKNPRKCNVVVTQPDTPPGS</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -804,14 +804,14 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LICVKEKFLFSETTETCPDGQNVCFNQAHLIYPGKYKRTRGCAATCPKLQNRDVIFCCSTDKCNL</t>
+          <t>ITSVSWCTPGCTSEGGGSGCSHCC</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>